<commit_message>
Added a chart in 09_03.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/09_03.xlsx
+++ b/Exercise Files/09_03.xlsx
@@ -1,35 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yapatel/Desktop/ExerciseFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quintiles-my.sharepoint.com/personal/mdmuntaha_islam_iqvia_com/Documents/Documents/My Courses/Data-Analytics-for-Business-Professionals/Exercise Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_2E77F3DA211B8CAC1617B501A65FC10F6AF8D9DC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{697BC781-916C-4CE0-8093-0FF72894AC79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27400" windowHeight="11800" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRST" sheetId="20" r:id="rId1"/>
     <sheet name="FIRST GRAPH" sheetId="21" r:id="rId2"/>
-    <sheet name="SECOND" sheetId="22" r:id="rId3"/>
-    <sheet name="SECOND GRAPH" sheetId="23" r:id="rId4"/>
-    <sheet name="THIRD" sheetId="19" r:id="rId5"/>
-    <sheet name="Third Chart" sheetId="25" r:id="rId6"/>
-    <sheet name="FOURTH" sheetId="24" r:id="rId7"/>
+    <sheet name="My Version of First Graph" sheetId="26" r:id="rId3"/>
+    <sheet name="SECOND" sheetId="22" r:id="rId4"/>
+    <sheet name="SECOND GRAPH" sheetId="23" r:id="rId5"/>
+    <sheet name="THIRD" sheetId="19" r:id="rId6"/>
+    <sheet name="Third Chart" sheetId="25" r:id="rId7"/>
+    <sheet name="FOURTH" sheetId="24" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -134,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -309,7 +320,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -435,21 +446,21 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2500.0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>750.0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0F4D-4DB4-8FC9-85B89C783182}"/>
             </c:ext>
@@ -526,22 +537,22 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>32500.0</c:v>
+                  <c:v>32500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26500.0</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14200.0</c:v>
+                  <c:v>14200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13000.0</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0F4D-4DB4-8FC9-85B89C783182}"/>
             </c:ext>
@@ -559,7 +570,7 @@
         <c:smooth val="0"/>
         <c:axId val="-1388506512"/>
         <c:axId val="-1469662832"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -567,7 +578,7 @@
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$3</c15:sqref>
@@ -605,7 +616,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -631,7 +642,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                    <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$3:$F$3</c15:sqref>
@@ -645,7 +656,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -658,7 +669,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$4</c15:sqref>
@@ -699,7 +710,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -725,7 +736,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$4:$F$4</c15:sqref>
@@ -736,22 +747,22 @@
                       <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>500.0</c:v>
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>500.0</c:v>
+                        <c:v>500</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>2200.0</c:v>
+                        <c:v>2200</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2000.0</c:v>
+                        <c:v>2000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -764,7 +775,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$6</c15:sqref>
@@ -805,7 +816,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -831,7 +842,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$6:$F$6</c15:sqref>
@@ -842,22 +853,22 @@
                       <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>3000.0</c:v>
+                        <c:v>3000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2500.0</c:v>
+                        <c:v>2500</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3000.0</c:v>
+                        <c:v>3000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2750.0</c:v>
+                        <c:v>2750</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -870,7 +881,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$7</c15:sqref>
@@ -908,7 +919,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -934,7 +945,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$7:$F$7</c15:sqref>
@@ -948,7 +959,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -961,7 +972,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$8</c15:sqref>
@@ -999,7 +1010,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1025,7 +1036,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$8:$F$8</c15:sqref>
@@ -1039,7 +1050,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1052,7 +1063,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$9</c15:sqref>
@@ -1099,7 +1110,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1125,7 +1136,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$9:$F$9</c15:sqref>
@@ -1136,22 +1147,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>12500.0</c:v>
+                        <c:v>12500</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>12500.0</c:v>
+                        <c:v>12500</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>55000.0</c:v>
+                        <c:v>55000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>50000.0</c:v>
+                        <c:v>50000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1164,7 +1175,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$10</c15:sqref>
@@ -1211,7 +1222,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1237,7 +1248,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$10:$F$10</c15:sqref>
@@ -1248,22 +1259,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>100000.0</c:v>
+                        <c:v>100000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>80000.0</c:v>
+                        <c:v>80000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>32000.0</c:v>
+                        <c:v>32000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>30000.0</c:v>
+                        <c:v>30000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1276,7 +1287,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$11</c15:sqref>
@@ -1323,7 +1334,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1349,7 +1360,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$11:$F$11</c15:sqref>
@@ -1360,22 +1371,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>112500.0</c:v>
+                        <c:v>112500</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>92500.0</c:v>
+                        <c:v>92500</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>87000.0</c:v>
+                        <c:v>87000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>80000.0</c:v>
+                        <c:v>80000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1388,7 +1399,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$12</c15:sqref>
@@ -1432,7 +1443,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1458,7 +1469,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$12:$F$12</c15:sqref>
@@ -1472,7 +1483,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1485,7 +1496,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$13</c15:sqref>
@@ -1532,7 +1543,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1558,7 +1569,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$13:$F$13</c15:sqref>
@@ -1569,22 +1580,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>10000.0</c:v>
+                        <c:v>10000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10000.0</c:v>
+                        <c:v>10000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>44000.0</c:v>
+                        <c:v>44000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>40000.0</c:v>
+                        <c:v>40000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1597,7 +1608,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$14</c15:sqref>
@@ -1644,7 +1655,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1670,7 +1681,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$14:$F$14</c15:sqref>
@@ -1681,22 +1692,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>70000.0</c:v>
+                        <c:v>70000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>56000.0</c:v>
+                        <c:v>56000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>28800.0</c:v>
+                        <c:v>28800</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>27000.0</c:v>
+                        <c:v>27000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1709,7 +1720,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$15</c15:sqref>
@@ -1759,7 +1770,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1785,7 +1796,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$15:$F$15</c15:sqref>
@@ -1796,22 +1807,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>80000.0</c:v>
+                        <c:v>80000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>66000.0</c:v>
+                        <c:v>66000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>72800.0</c:v>
+                        <c:v>72800</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>67000.0</c:v>
+                        <c:v>67000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1824,7 +1835,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$16</c15:sqref>
@@ -1871,7 +1882,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -1897,7 +1908,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$16:$F$16</c15:sqref>
@@ -1911,7 +1922,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000E-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -1924,7 +1935,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$17</c15:sqref>
@@ -1974,7 +1985,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -2000,7 +2011,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$17:$F$17</c15:sqref>
@@ -2011,22 +2022,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>2500.0</c:v>
+                        <c:v>2500</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2500.0</c:v>
+                        <c:v>2500</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>11000.0</c:v>
+                        <c:v>11000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>10000.0</c:v>
+                        <c:v>10000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -2039,7 +2050,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$B$18</c15:sqref>
@@ -2089,7 +2100,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$2:$F$2</c15:sqref>
@@ -2115,7 +2126,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>FIRST!$C$18:$F$18</c15:sqref>
@@ -2126,22 +2137,22 @@
                       <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                       <c:ptCount val="4"/>
                       <c:pt idx="0">
-                        <c:v>30000.0</c:v>
+                        <c:v>30000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>24000.0</c:v>
+                        <c:v>24000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3200.0</c:v>
+                        <c:v>3200</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>3000.0</c:v>
+                        <c:v>3000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-0F4D-4DB4-8FC9-85B89C783182}"/>
                   </c:ext>
@@ -2390,7 +2401,439 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FIRST!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Long Sleeved Shirt Units</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>FIRST!$C$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC48-4BE8-BF61-A0D1CC899263}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="738717152"/>
+        <c:axId val="738713872"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FIRST!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Profits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>FIRST!$C$19:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AC48-4BE8-BF61-A0D1CC899263}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="741083168"/>
+        <c:axId val="741084152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="738717152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="738713872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="738713872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="738717152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="741084152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="741083168"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="741083168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="741084152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2500,30 +2943,30 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750.0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2500.0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>750.0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D717-4D79-A843-67C1FBC62D7F}"/>
             </c:ext>
@@ -2609,31 +3052,31 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>26500.0</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14800.0</c:v>
+                  <c:v>14800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19000.0</c:v>
+                  <c:v>19000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32500.0</c:v>
+                  <c:v>32500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26500.0</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14200.0</c:v>
+                  <c:v>14200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13000.0</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D717-4D79-A843-67C1FBC62D7F}"/>
             </c:ext>
@@ -2890,8 +3333,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2980,7 +3423,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-A885-4B05-9B73-43362C4F8F6A}"/>
               </c:ext>
@@ -3025,33 +3468,33 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>750.0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2500.0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>800.0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>750.0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2500.0</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A885-4B05-9B73-43362C4F8F6A}"/>
             </c:ext>
@@ -3137,34 +3580,34 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>26500.0</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14800.0</c:v>
+                  <c:v>14800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19000.0</c:v>
+                  <c:v>19000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32500.0</c:v>
+                  <c:v>32500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26500.0</c:v>
+                  <c:v>26500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14200.0</c:v>
+                  <c:v>14200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13000.0</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12500.0</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A885-4B05-9B73-43362C4F8F6A}"/>
             </c:ext>
@@ -3541,6 +3984,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4058,7 +4541,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4166,11 +4649,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4181,11 +4659,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4217,9 +4690,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5089,11 +5559,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5101,7 +6087,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
@@ -5112,7 +6098,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0" zoomToFit="1"/>
@@ -5126,13 +6112,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656285" cy="6283854"/>
+    <xdr:ext cx="8661797" cy="6290469"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6AFF086A-DF4C-422C-A2A3-FCADE419008B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AFF086A-DF4C-422C-A2A3-FCADE419008B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5157,6 +6143,49 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B7816FD-C135-41D4-800F-0EE7F12B610D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8656285" cy="6283854"/>
@@ -5165,7 +6194,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{028BBB93-9AC2-4C0F-9E3D-40A95CCB886D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028BBB93-9AC2-4C0F-9E3D-40A95CCB886D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5188,7 +6217,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -5198,7 +6227,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26313B46-FE13-4162-9B4E-A02929F5B21B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26313B46-FE13-4162-9B4E-A02929F5B21B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5517,22 +6546,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" activeCellId="1" sqref="B5:F5 B19:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="6" width="11.6328125" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -5541,7 +6570,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" t="s">
         <v>14</v>
@@ -5559,7 +6588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5579,7 +6608,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -5596,7 +6625,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -5617,7 +6646,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -5637,7 +6666,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -5654,7 +6683,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5675,10 +6704,10 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -5698,7 +6727,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -5715,7 +6744,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
@@ -5736,7 +6765,7 @@
         <v>67000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5756,7 +6785,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>25</v>
       </c>
@@ -5773,7 +6802,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
@@ -5794,7 +6823,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -5807,25 +6836,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB873281-9C4B-4E9A-8917-E514083EC948}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="9" width="11.6328125" customWidth="1"/>
+    <col min="10" max="10" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -5835,7 +6877,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -5864,7 +6906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5893,7 +6935,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -5919,7 +6961,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -5952,7 +6994,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -5981,7 +7023,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -6007,7 +7049,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
@@ -6040,10 +7082,10 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -6072,7 +7114,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -6098,7 +7140,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -6131,7 +7173,7 @@
         <v>67000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -6160,7 +7202,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -6186,7 +7228,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
@@ -6219,7 +7261,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -6234,26 +7276,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="10" width="11.6328125" customWidth="1"/>
+    <col min="11" max="11" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -6264,7 +7306,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
@@ -6296,7 +7338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
@@ -6328,7 +7370,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>19</v>
@@ -6358,7 +7400,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="23" t="s">
         <v>15</v>
@@ -6396,7 +7438,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -6408,7 +7450,7 @@
       <c r="I6" s="17"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
@@ -6440,7 +7482,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -6470,7 +7512,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="23" t="s">
         <v>16</v>
@@ -6508,7 +7550,7 @@
         <v>112500</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
       <c r="B10" s="23"/>
       <c r="C10" s="17"/>
@@ -6520,7 +7562,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="35"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>2</v>
       </c>
@@ -6552,7 +7594,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>23</v>
@@ -6582,7 +7624,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="17"/>
       <c r="B13" s="23" t="s">
         <v>17</v>
@@ -6620,7 +7662,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -6632,7 +7674,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="35"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>7</v>
       </c>
@@ -6664,7 +7706,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>25</v>
@@ -6694,7 +7736,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="17"/>
       <c r="B17" s="23" t="s">
         <v>13</v>
@@ -6732,7 +7774,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="29"/>
@@ -6750,26 +7792,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="10" width="11.6328125" customWidth="1"/>
+    <col min="11" max="11" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="17"/>
       <c r="C1" s="23"/>
@@ -6781,7 +7823,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -6813,7 +7855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6845,7 +7887,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
         <v>19</v>
       </c>
@@ -6874,7 +7916,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
         <v>15</v>
       </c>
@@ -6911,7 +7953,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -6922,7 +7964,7 @@
       <c r="I6" s="17"/>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -6954,7 +7996,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="17" t="s">
         <v>21</v>
       </c>
@@ -6983,7 +8025,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
         <v>16</v>
       </c>
@@ -7020,7 +8062,7 @@
         <v>112500</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="23"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -7031,7 +8073,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -7063,7 +8105,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
         <v>23</v>
       </c>
@@ -7092,7 +8134,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
         <v>17</v>
       </c>
@@ -7129,7 +8171,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -7140,7 +8182,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="24"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -7172,7 +8214,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="17" t="s">
         <v>25</v>
       </c>
@@ -7201,7 +8243,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
         <v>13</v>
       </c>
@@ -7238,7 +8280,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B18" s="17"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
@@ -7249,7 +8291,7 @@
       <c r="I18" s="29"/>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>29</v>
       </c>

</xml_diff>